<commit_message>
Created ClueLayout.csv, ClueSetup.txt, and readme.txt
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carte\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFAD158-E7A0-445A-A4F3-950DF348F1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44AF22D2-0855-4C7D-B088-141AE3E9F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,58 +36,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="37">
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>K*</t>
+  </si>
+  <si>
+    <t>G*</t>
+  </si>
+  <si>
+    <t>D*</t>
+  </si>
+  <si>
+    <t>K#</t>
+  </si>
+  <si>
+    <t>G#</t>
+  </si>
+  <si>
+    <t>D#</t>
+  </si>
+  <si>
+    <t>W&gt;</t>
+  </si>
+  <si>
+    <t>W^</t>
+  </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>W^</t>
-  </si>
-  <si>
-    <t>W&gt;</t>
+    <t>Wv</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>H*</t>
+  </si>
+  <si>
+    <t>P*</t>
+  </si>
+  <si>
+    <t>H#</t>
+  </si>
+  <si>
+    <t>W&lt;</t>
+  </si>
+  <si>
+    <t>P#</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Wv</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>W&lt;</t>
+    <t>O*</t>
+  </si>
+  <si>
+    <t>O#</t>
+  </si>
+  <si>
+    <t>L*</t>
+  </si>
+  <si>
+    <t>T*</t>
+  </si>
+  <si>
+    <t>S*</t>
+  </si>
+  <si>
+    <t>L#</t>
+  </si>
+  <si>
+    <t>T#</t>
+  </si>
+  <si>
+    <t>S#</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,12 +170,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,98 +196,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -313,136 +302,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -793,15 +652,15 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="27" width="3.77734375" customWidth="1"/>
+    <col min="1" max="27" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -906,12 +765,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -985,11 +844,11 @@
       <c r="Z2" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" t="s">
-        <v>4</v>
+      <c r="AA2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -1073,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="3">A3+1</f>
         <v>2</v>
@@ -1145,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="X4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
@@ -1157,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1169,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -1199,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O5" t="s">
         <v>3</v>
@@ -1232,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="Y5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Z5" t="s">
         <v>4</v>
@@ -1241,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1256,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
@@ -1286,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="O6" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="P6" t="s">
         <v>3</v>
@@ -1325,7 +1184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1409,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1493,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1526,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>
@@ -1556,7 +1415,7 @@
         <v>2</v>
       </c>
       <c r="U9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="V9" t="s">
         <v>4</v>
@@ -1577,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1598,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
         <v>2</v>
@@ -1661,16 +1520,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -1745,16 +1604,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -1790,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="O12" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="P12" t="s">
         <v>2</v>
@@ -1811,49 +1670,49 @@
         <v>2</v>
       </c>
       <c r="V12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="W12" t="s">
         <v>2</v>
       </c>
       <c r="X12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
         <v>2</v>
@@ -1889,166 +1748,166 @@
         <v>2</v>
       </c>
       <c r="T13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I14" t="s">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q14" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R14" t="s">
         <v>2</v>
       </c>
       <c r="S14" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q15" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R15" t="s">
         <v>2</v>
@@ -2057,82 +1916,82 @@
         <v>2</v>
       </c>
       <c r="T15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W15" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="X15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R16" t="s">
         <v>2</v>
@@ -2141,82 +2000,82 @@
         <v>2</v>
       </c>
       <c r="T16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X16" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="Y16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27">
       <c r="A17" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q17" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R17" t="s">
         <v>2</v>
@@ -2225,166 +2084,166 @@
         <v>2</v>
       </c>
       <c r="T17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA17" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27">
       <c r="A18" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q18" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R18" t="s">
         <v>2</v>
       </c>
       <c r="S18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s">
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R19" t="s">
         <v>2</v>
@@ -2393,46 +2252,46 @@
         <v>2</v>
       </c>
       <c r="T19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="V19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="X19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA19" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -2483,34 +2342,34 @@
         <v>2</v>
       </c>
       <c r="V20" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="W20" t="s">
         <v>2</v>
       </c>
       <c r="X20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AA20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -2534,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="K21" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="L21" t="s">
         <v>2</v>
@@ -2585,25 +2444,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
         <v>2</v>
@@ -2615,13 +2474,13 @@
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L22" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M22" t="s">
         <v>2</v>
@@ -2636,7 +2495,7 @@
         <v>2</v>
       </c>
       <c r="Q22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="R22" t="s">
         <v>2</v>
@@ -2669,22 +2528,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s">
         <v>2</v>
@@ -2693,40 +2552,40 @@
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M23" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N23" t="s">
         <v>2</v>
       </c>
       <c r="O23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T23" t="s">
         <v>2</v>
@@ -2738,37 +2597,37 @@
         <v>2</v>
       </c>
       <c r="W23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -2777,40 +2636,40 @@
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M24" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N24" t="s">
         <v>2</v>
       </c>
       <c r="O24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T24" t="s">
         <v>2</v>
@@ -2819,40 +2678,40 @@
         <v>2</v>
       </c>
       <c r="V24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="W24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
         <v>2</v>
@@ -2861,40 +2720,40 @@
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="O25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T25" t="s">
         <v>2</v>
@@ -2903,40 +2762,40 @@
         <v>2</v>
       </c>
       <c r="V25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA25" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27">
       <c r="A26" s="1">
         <f>A25+1</f>
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
         <v>2</v>
@@ -2945,40 +2804,40 @@
         <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="K26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N26" t="s">
         <v>2</v>
       </c>
       <c r="O26" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P26" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q26" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="R26" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S26" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T26" t="s">
         <v>2</v>
@@ -2987,40 +2846,40 @@
         <v>2</v>
       </c>
       <c r="V26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X26" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="Y26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27">
       <c r="A27" s="1">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
@@ -3029,40 +2888,40 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K27" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="L27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N27" t="s">
         <v>2</v>
       </c>
       <c r="O27" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P27" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q27" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="R27" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S27" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T27" t="s">
         <v>2</v>
@@ -3071,82 +2930,82 @@
         <v>2</v>
       </c>
       <c r="V27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y27" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="Z27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" t="s">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" t="s">
-        <v>6</v>
-      </c>
       <c r="O28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T28" t="s">
         <v>2</v>
@@ -3155,40 +3014,40 @@
         <v>2</v>
       </c>
       <c r="V28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
         <v>2</v>
@@ -3197,40 +3056,40 @@
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N29" t="s">
         <v>2</v>
       </c>
       <c r="O29" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P29" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q29" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R29" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S29" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T29" t="s">
         <v>2</v>
@@ -3239,40 +3098,40 @@
         <v>2</v>
       </c>
       <c r="V29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AA29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27">
       <c r="A30" s="1">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>12</v>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
         <v>2</v>
@@ -3281,40 +3140,40 @@
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N30" t="s">
         <v>2</v>
       </c>
       <c r="O30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="Q30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T30" t="s">
         <v>2</v>
@@ -3323,64 +3182,64 @@
         <v>2</v>
       </c>
       <c r="V30" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="W30" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X30" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y30" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Z30" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="AA30" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AA30">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added the Test.txt and changed the tests to match are board
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carte\CSCI306\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44AF22D2-0855-4C7D-B088-141AE3E9F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2330B5C2-5F63-41BF-976A-08420416F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="18010" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +205,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -296,16 +303,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF7030A0"/>
@@ -313,9 +310,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF7030A0"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -652,15 +652,15 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="AF15" sqref="AF15"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="27" width="3.7109375" customWidth="1"/>
+    <col min="1" max="27" width="3.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -765,7 +765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="3">A3+1</f>
         <v>2</v>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1184,7 +1184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1268,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1352,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1436,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1520,7 +1520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1604,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1688,7 +1688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1772,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1856,7 +1856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1940,7 +1940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2024,7 +2024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -2108,7 +2108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -2192,7 +2192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -2276,7 +2276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -2360,7 +2360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -2444,7 +2444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -2528,7 +2528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2612,7 +2612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -2696,7 +2696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -2780,7 +2780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f>A25+1</f>
         <v>24</v>
@@ -2864,7 +2864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -2948,7 +2948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3032,7 +3032,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3116,7 +3116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -3201,46 +3201,46 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="A1:AA30">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA30">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"X"</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>"W"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"L"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"K"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+      <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>"K"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"S"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"T"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"L"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"O"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"H"</formula>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created BoardAdjTargetTest.java did Adj room, doors, walkways also did calctargets test on Royal Dining Room and Spa
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2330B5C2-5F63-41BF-976A-08420416F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593775F-9BE1-4F67-B740-9FB07E975902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18010" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="43">
   <si>
     <t>GS</t>
   </si>
@@ -147,13 +147,31 @@
   </si>
   <si>
     <t>SG</t>
+  </si>
+  <si>
+    <t>Number of doors: 17</t>
+  </si>
+  <si>
+    <t>white: door direction tests (fileinit)</t>
+  </si>
+  <si>
+    <t>Grey: room test (flileInit)</t>
+  </si>
+  <si>
+    <t>Light Orange: adjacency from room and doors</t>
+  </si>
+  <si>
+    <t>Dark  Orange: adjacent walkways</t>
+  </si>
+  <si>
+    <t>Light blue: test targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +187,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +218,58 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,18 +283,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="84">
     <dxf>
       <fill>
         <patternFill>
@@ -214,91 +323,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,11 +340,763 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -649,18 +1430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D044B7-EFD5-4F17-94B4-AF279085F3A6}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="27" width="3.7265625" customWidth="1"/>
+    <col min="28" max="28" width="38.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -764,8 +1546,11 @@
         <f t="shared" ref="AA1" si="2">Z1+1</f>
         <v>25</v>
       </c>
+      <c r="AB1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -787,7 +1572,7 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
@@ -847,8 +1632,11 @@
       <c r="AA2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="AB2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -931,8 +1719,11 @@
       <c r="AA3" t="s">
         <v>4</v>
       </c>
+      <c r="AB3" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="3">A3+1</f>
         <v>2</v>
@@ -1003,7 +1794,7 @@
       <c r="W4" t="s">
         <v>4</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="Y4" t="s">
@@ -1015,8 +1806,9 @@
       <c r="AA4" t="s">
         <v>4</v>
       </c>
+      <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1027,7 +1819,7 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
@@ -1057,7 +1849,7 @@
       <c r="M5" t="s">
         <v>3</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="O5" t="s">
@@ -1090,7 +1882,7 @@
       <c r="X5" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Y5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="Z5" t="s">
@@ -1099,8 +1891,11 @@
       <c r="AA5" t="s">
         <v>4</v>
       </c>
+      <c r="AB5" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1114,7 +1909,7 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
@@ -1144,7 +1939,7 @@
       <c r="N6" t="s">
         <v>3</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P6" t="s">
@@ -1183,8 +1978,11 @@
       <c r="AA6" t="s">
         <v>4</v>
       </c>
+      <c r="AB6" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1267,8 +2065,11 @@
       <c r="AA7" t="s">
         <v>4</v>
       </c>
+      <c r="AB7" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1352,7 +2153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1414,7 +2215,7 @@
       <c r="T9" t="s">
         <v>2</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="V9" t="s">
@@ -1436,7 +2237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1456,7 +2257,7 @@
       <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H10" t="s">
@@ -1520,7 +2321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1582,7 +2383,7 @@
       <c r="T11" t="s">
         <v>2</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="V11" t="s">
@@ -1604,7 +2405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1648,7 +2449,7 @@
       <c r="N12" t="s">
         <v>2</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="P12" t="s">
@@ -1660,13 +2461,13 @@
       <c r="R12" t="s">
         <v>2</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T12" t="s">
         <v>2</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="V12" t="s">
@@ -1688,7 +2489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1744,7 +2545,7 @@
       <c r="R13" t="s">
         <v>2</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T13" t="s">
@@ -1772,7 +2573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1828,7 +2629,7 @@
       <c r="R14" t="s">
         <v>2</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="T14" t="s">
@@ -1837,16 +2638,16 @@
       <c r="U14" t="s">
         <v>16</v>
       </c>
-      <c r="V14" t="s">
-        <v>16</v>
-      </c>
-      <c r="W14" t="s">
-        <v>16</v>
-      </c>
-      <c r="X14" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y14" t="s">
+      <c r="V14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="Z14" t="s">
@@ -1856,7 +2657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1864,13 +2665,13 @@
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F15" t="s">
@@ -1882,7 +2683,7 @@
       <c r="H15" t="s">
         <v>17</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="13" t="s">
         <v>2</v>
       </c>
       <c r="J15" t="s">
@@ -1912,7 +2713,7 @@
       <c r="R15" t="s">
         <v>2</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T15" t="s">
@@ -1921,16 +2722,16 @@
       <c r="U15" t="s">
         <v>16</v>
       </c>
-      <c r="V15" t="s">
-        <v>16</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="V15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="X15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y15" t="s">
+      <c r="X15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="Z15" t="s">
@@ -1940,7 +2741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1948,13 +2749,13 @@
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F16" t="s">
@@ -1996,7 +2797,7 @@
       <c r="R16" t="s">
         <v>2</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T16" t="s">
@@ -2005,16 +2806,16 @@
       <c r="U16" t="s">
         <v>16</v>
       </c>
-      <c r="V16" t="s">
-        <v>16</v>
-      </c>
-      <c r="W16" t="s">
-        <v>16</v>
-      </c>
-      <c r="X16" t="s">
+      <c r="V16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Y16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="Z16" t="s">
@@ -2050,7 +2851,7 @@
       <c r="H17" t="s">
         <v>17</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J17" t="s">
@@ -2080,7 +2881,7 @@
       <c r="R17" t="s">
         <v>2</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T17" t="s">
@@ -2134,7 +2935,7 @@
       <c r="H18" t="s">
         <v>17</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J18" t="s">
@@ -2164,7 +2965,7 @@
       <c r="R18" t="s">
         <v>2</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="T18" t="s">
@@ -2290,7 +3091,7 @@
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
@@ -2338,10 +3139,10 @@
       <c r="T20" t="s">
         <v>2</v>
       </c>
-      <c r="U20" t="s">
-        <v>2</v>
-      </c>
-      <c r="V20" t="s">
+      <c r="U20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="W20" t="s">
@@ -2392,7 +3193,7 @@
       <c r="J21" t="s">
         <v>2</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L21" t="s">
@@ -2422,10 +3223,10 @@
       <c r="T21" t="s">
         <v>2</v>
       </c>
-      <c r="U21" t="s">
-        <v>2</v>
-      </c>
-      <c r="V21" t="s">
+      <c r="U21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="W21" t="s">
@@ -2461,7 +3262,7 @@
       <c r="E22" t="s">
         <v>23</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G22" t="s">
@@ -2488,13 +3289,13 @@
       <c r="N22" t="s">
         <v>2</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="P22" t="s">
         <v>2</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="12" t="s">
         <v>15</v>
       </c>
       <c r="R22" t="s">
@@ -2653,7 +3454,7 @@
       <c r="M24" t="s">
         <v>24</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O24" t="s">
@@ -2677,7 +3478,7 @@
       <c r="U24" t="s">
         <v>2</v>
       </c>
-      <c r="V24" t="s">
+      <c r="V24" s="12" t="s">
         <v>15</v>
       </c>
       <c r="W24" t="s">
@@ -2704,7 +3505,7 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D25" t="s">
@@ -2737,7 +3538,7 @@
       <c r="M25" t="s">
         <v>24</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="O25" t="s">
@@ -2746,7 +3547,7 @@
       <c r="P25" t="s">
         <v>25</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="8" t="s">
         <v>25</v>
       </c>
       <c r="R25" t="s">
@@ -2770,7 +3571,7 @@
       <c r="X25" t="s">
         <v>26</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Y25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="Z25" t="s">
@@ -2791,7 +3592,7 @@
       <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E26" t="s">
@@ -2809,7 +3610,7 @@
       <c r="I26" t="s">
         <v>24</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="6" t="s">
         <v>29</v>
       </c>
       <c r="K26" t="s">
@@ -2821,7 +3622,7 @@
       <c r="M26" t="s">
         <v>24</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O26" t="s">
@@ -2830,7 +3631,7 @@
       <c r="P26" t="s">
         <v>25</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="8" t="s">
         <v>30</v>
       </c>
       <c r="R26" t="s">
@@ -2851,7 +3652,7 @@
       <c r="W26" t="s">
         <v>26</v>
       </c>
-      <c r="X26" t="s">
+      <c r="X26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="Y26" t="s">
@@ -2896,7 +3697,7 @@
       <c r="J27" t="s">
         <v>24</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L27" t="s">
@@ -2905,7 +3706,7 @@
       <c r="M27" t="s">
         <v>24</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O27" t="s">
@@ -2914,7 +3715,7 @@
       <c r="P27" t="s">
         <v>25</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="R27" t="s">
@@ -2938,7 +3739,7 @@
       <c r="X27" t="s">
         <v>26</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Y27" s="8" t="s">
         <v>34</v>
       </c>
       <c r="Z27" t="s">
@@ -2989,7 +3790,7 @@
       <c r="M28" t="s">
         <v>24</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O28" t="s">
@@ -2998,7 +3799,7 @@
       <c r="P28" t="s">
         <v>25</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="Q28" s="8" t="s">
         <v>25</v>
       </c>
       <c r="R28" t="s">
@@ -3073,7 +3874,7 @@
       <c r="M29" t="s">
         <v>24</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O29" t="s">
@@ -3157,7 +3958,7 @@
       <c r="M30" t="s">
         <v>24</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O30" t="s">
@@ -3201,45 +4002,45 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AA30">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:AA1 A26:AA29 A25:X25 Z25:AA25 A3:AA14 A2:G2 I2:AA2 A30:M30 O30:AA30 A16:AA21 A15:H15 J15:AA15 A23:AA24 A22:N22 P22:AA22">
+    <cfRule type="cellIs" dxfId="71" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A26:XFD29 A25:X25 Z25:XFD25 A3:XFD14 A2:G2 I2:XFD2 A31:XFD1048576 A30:M30 O30:XFD30 A16:XFD21 A15:H15 J15:XFD15 A23:XFD24 A22:N22 P22:XFD22">
+    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed test targets (AtDoor,Walkway1,Walkway2,Occupied) in BoardAdjTargetTest class and marked cells in excel sheet.
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carte\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593775F-9BE1-4F67-B740-9FB07E975902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1C9520-0066-4EB2-8422-812911A14F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <t>Dark  Orange: adjacent walkways</t>
   </si>
   <si>
-    <t>Light blue: test targets</t>
+    <t>Light blue: test targets, P* (row=13,col=21) as well</t>
   </si>
 </sst>
 </file>
@@ -313,24 +313,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <fill>
         <patternFill>
@@ -425,23 +408,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -585,23 +551,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -704,399 +653,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1433,16 +989,16 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="27" width="3.7265625" customWidth="1"/>
-    <col min="28" max="28" width="38.1796875" customWidth="1"/>
+    <col min="1" max="27" width="3.77734375" customWidth="1"/>
+    <col min="28" max="28" width="42.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1550,7 +1106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1636,7 +1192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -1723,7 +1279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="3">A3+1</f>
         <v>2</v>
@@ -1808,7 +1364,7 @@
       </c>
       <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1895,7 +1451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1982,7 +1538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -2069,7 +1625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -2153,7 +1709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2237,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -2321,7 +1877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -2405,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -2470,7 +2026,7 @@
       <c r="U12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="W12" t="s">
@@ -2489,7 +2045,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -2573,7 +2129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -2657,7 +2213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2741,7 +2297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2825,7 +2381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -2909,7 +2465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -2993,7 +2549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -3077,7 +2633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -3161,7 +2717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -3175,7 +2731,7 @@
       <c r="D21" t="s">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F21" t="s">
@@ -3217,7 +2773,7 @@
       <c r="R21" t="s">
         <v>2</v>
       </c>
-      <c r="S21" t="s">
+      <c r="S21" s="14" t="s">
         <v>2</v>
       </c>
       <c r="T21" t="s">
@@ -3245,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -3329,7 +2885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -3413,7 +2969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -3497,7 +3053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -3581,7 +3137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f>A25+1</f>
         <v>24</v>
@@ -3665,7 +3221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -3749,7 +3305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3833,7 +3389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3917,7 +3473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -4002,45 +3558,45 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AA1 A26:AA29 A25:X25 Z25:AA25 A3:AA14 A2:G2 I2:AA2 A30:M30 O30:AA30 A16:AA21 A15:H15 J15:AA15 A23:AA24 A22:N22 P22:AA22">
-    <cfRule type="cellIs" dxfId="71" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA20 A22:N22 P22:AA22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30 A21:D21 F21:R21 T21:AA21">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A26:XFD29 A25:X25 Z25:XFD25 A3:XFD14 A2:G2 I2:XFD2 A31:XFD1048576 A30:M30 O30:XFD30 A16:XFD21 A15:H15 J15:XFD15 A23:XFD24 A22:N22 P22:XFD22">
-    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD20 A22:N22 P22:XFD22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576 A21:D21 F21:R21 T21:XFD21">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="83" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changed some of the tests up to fit are board
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carte\CSCI306\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1C9520-0066-4EB2-8422-812911A14F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF62B9A-8F1C-4D66-83BA-007553F49A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="44">
   <si>
     <t>GS</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Light blue: test targets, P* (row=13,col=21) as well</t>
+  </si>
+  <si>
+    <t>Red: Test Ocupied (P* as well )</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +276,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -307,6 +322,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -989,16 +1007,16 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="27" width="3.77734375" customWidth="1"/>
-    <col min="28" max="28" width="42.77734375" customWidth="1"/>
+    <col min="1" max="27" width="3.81640625" customWidth="1"/>
+    <col min="28" max="28" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1106,11 +1124,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -1185,14 +1203,14 @@
       <c r="Z2" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="AB2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -1279,7 +1297,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="3">A3+1</f>
         <v>2</v>
@@ -1364,7 +1382,7 @@
       </c>
       <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1451,7 +1469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1538,7 +1556,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1625,7 +1643,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1708,8 +1726,11 @@
       <c r="AA8" t="s">
         <v>4</v>
       </c>
+      <c r="AB8" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1771,7 +1792,7 @@
       <c r="T9" t="s">
         <v>2</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="U9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="V9" t="s">
@@ -1792,8 +1813,9 @@
       <c r="AA9" t="s">
         <v>4</v>
       </c>
+      <c r="AB9" s="18"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1877,7 +1899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1961,7 +1983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -2045,7 +2067,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -2129,7 +2151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -2213,7 +2235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2297,7 +2319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2381,7 +2403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -2465,7 +2487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -2549,7 +2571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -2602,7 +2624,7 @@
       <c r="Q19" t="s">
         <v>14</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="S19" t="s">
@@ -2633,7 +2655,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -2717,7 +2739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -2801,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -2857,7 +2879,7 @@
       <c r="R22" t="s">
         <v>2</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T22" t="s">
@@ -2885,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2969,7 +2991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -3053,7 +3075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -3137,7 +3159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f>A25+1</f>
         <v>24</v>
@@ -3221,7 +3243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -3305,7 +3327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3389,7 +3411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3473,12 +3495,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C30" t="s">
@@ -3553,50 +3575,50 @@
       <c r="Z30" t="s">
         <v>26</v>
       </c>
-      <c r="AA30" s="2" t="s">
+      <c r="AA30" s="16" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA20 A22:N22 P22:AA22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30 A21:D21 F21:R21 T21:AA21">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA18 A21:D21 F21:R21 A22:N22 P22:R22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30 T21:AA22 A20:AA20 A19:Q19 S19:AA19">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD20 A22:N22 P22:XFD22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576 A21:D21 F21:R21 T21:XFD21">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD18 A21:D21 F21:R21 A22:N22 P22:R22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576 T21:XFD22 A20:XFD20 A19:Q19 S19:XFD19">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
got all adj list tests to pass
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF62B9A-8F1C-4D66-83BA-007553F49A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF48BCF9-EE29-43E0-8783-0E03959F5E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="18010" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,235 +331,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1007,7 +779,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3580,45 +3352,45 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA18 A21:D21 F21:R21 A22:N22 P22:R22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30 T21:AA22 A20:AA20 A19:Q19 S19:AA19">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA18 A19:Q19 S19:AA19 A20:AA20 A21:D21 F21:R21 T21:AA22 A22:N22 P22:R22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD18 A21:D21 F21:R21 A22:N22 P22:R22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576 T21:XFD22 A20:XFD20 A19:Q19 S19:XFD19">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD18 A19:Q19 S19:XFD19 A20:XFD20 A21:D21 F21:R21 T21:XFD22 A22:N22 P22:R22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
All test now pass :)
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B23BC7C-B414-4AA1-A3DA-75330E41FD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CFCB50-EF69-4A05-9E82-E224BC20BBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18010" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="18280" windowHeight="19730" xr2:uid="{9C97CBFD-98D6-42DB-B95D-9548993877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,121 +331,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -893,7 +779,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3467,44 +3353,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AA1 A2:G2 I2:AA2 A3:AA14 A15:H15 J15:AA15 A16:AA18 A19:Q19 T19:AA19 A20:AA20 A21:D21 F21:R21 T21:AA22 A22:N22 P22:R22 A23:AA24 A25:X25 Z25:AA25 A26:AA29 A30:M30 O30:AA30">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A2:G2 I2:XFD2 A3:XFD14 A15:H15 J15:XFD15 A16:XFD18 A19:Q19 T19:XFD19 A20:XFD20 A21:D21 F21:R21 T21:XFD22 A22:N22 P22:R22 A23:XFD24 A25:X25 Z25:XFD25 A26:XFD29 A30:M30 O30:XFD30 A31:XFD1048576">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"K"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>